<commit_message>
Refactor UI with cursor glow effect
</commit_message>
<xml_diff>
--- a/events-bangalore.xlsx
+++ b/events-bangalore.xlsx
@@ -454,10 +454,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H2" t="str">
-        <v>2026-02-03T14:07:13.572Z</v>
+        <v>2026-02-03T14:49:20.046Z</v>
       </c>
       <c r="I2" t="str">
-        <v>2026-02-03T14:07:13.607Z</v>
+        <v>2026-02-03T14:49:20.075Z</v>
       </c>
     </row>
     <row r="3">
@@ -483,10 +483,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H3" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.047Z</v>
       </c>
       <c r="I3" t="str">
-        <v>2026-02-03T14:07:13.616Z</v>
+        <v>2026-02-03T14:49:20.082Z</v>
       </c>
     </row>
     <row r="4">
@@ -512,10 +512,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H4" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.047Z</v>
       </c>
       <c r="I4" t="str">
-        <v>2026-02-03T14:07:13.618Z</v>
+        <v>2026-02-03T14:49:20.084Z</v>
       </c>
     </row>
     <row r="5">
@@ -541,10 +541,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H5" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.047Z</v>
       </c>
       <c r="I5" t="str">
-        <v>2026-02-03T14:07:13.620Z</v>
+        <v>2026-02-03T14:49:20.087Z</v>
       </c>
     </row>
     <row r="6">
@@ -570,10 +570,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H6" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.047Z</v>
       </c>
       <c r="I6" t="str">
-        <v>2026-02-03T14:07:13.621Z</v>
+        <v>2026-02-03T14:49:20.095Z</v>
       </c>
     </row>
     <row r="7">
@@ -599,10 +599,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H7" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.048Z</v>
       </c>
       <c r="I7" t="str">
-        <v>2026-02-03T14:07:13.623Z</v>
+        <v>2026-02-03T14:49:20.097Z</v>
       </c>
     </row>
     <row r="8">
@@ -628,10 +628,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H8" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.048Z</v>
       </c>
       <c r="I8" t="str">
-        <v>2026-02-03T14:07:13.629Z</v>
+        <v>2026-02-03T14:49:20.101Z</v>
       </c>
     </row>
     <row r="9">
@@ -657,10 +657,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H9" t="str">
-        <v>2026-02-03T14:07:13.574Z</v>
+        <v>2026-02-03T14:49:20.048Z</v>
       </c>
       <c r="I9" t="str">
-        <v>2026-02-03T14:07:13.630Z</v>
+        <v>2026-02-03T14:49:20.104Z</v>
       </c>
     </row>
     <row r="10">
@@ -686,10 +686,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H10" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.048Z</v>
       </c>
       <c r="I10" t="str">
-        <v>2026-02-03T14:07:13.632Z</v>
+        <v>2026-02-03T14:49:20.107Z</v>
       </c>
     </row>
     <row r="11">
@@ -715,10 +715,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H11" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I11" t="str">
-        <v>2026-02-03T14:07:13.635Z</v>
+        <v>2026-02-03T14:49:20.111Z</v>
       </c>
     </row>
     <row r="12">
@@ -744,10 +744,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H12" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I12" t="str">
-        <v>2026-02-03T14:07:13.637Z</v>
+        <v>2026-02-03T14:49:20.118Z</v>
       </c>
     </row>
     <row r="13">
@@ -773,10 +773,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H13" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I13" t="str">
-        <v>2026-02-03T14:07:13.640Z</v>
+        <v>2026-02-03T14:49:20.122Z</v>
       </c>
     </row>
     <row r="14">
@@ -802,10 +802,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H14" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I14" t="str">
-        <v>2026-02-03T14:07:13.647Z</v>
+        <v>2026-02-03T14:49:20.124Z</v>
       </c>
     </row>
     <row r="15">
@@ -831,10 +831,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H15" t="str">
-        <v>2026-02-03T14:07:13.575Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I15" t="str">
-        <v>2026-02-03T14:07:13.649Z</v>
+        <v>2026-02-03T14:49:20.127Z</v>
       </c>
     </row>
     <row r="16">
@@ -860,10 +860,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H16" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I16" t="str">
-        <v>2026-02-03T14:07:13.651Z</v>
+        <v>2026-02-03T14:49:20.131Z</v>
       </c>
     </row>
     <row r="17">
@@ -889,10 +889,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H17" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I17" t="str">
-        <v>2026-02-03T14:07:13.654Z</v>
+        <v>2026-02-03T14:49:20.133Z</v>
       </c>
     </row>
     <row r="18">
@@ -918,10 +918,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H18" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I18" t="str">
-        <v>2026-02-03T14:07:13.657Z</v>
+        <v>2026-02-03T14:49:20.136Z</v>
       </c>
     </row>
     <row r="19">
@@ -947,10 +947,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H19" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.049Z</v>
       </c>
       <c r="I19" t="str">
-        <v>2026-02-03T14:07:13.660Z</v>
+        <v>2026-02-03T14:49:20.139Z</v>
       </c>
     </row>
     <row r="20">
@@ -976,10 +976,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H20" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I20" t="str">
-        <v>2026-02-03T14:07:13.663Z</v>
+        <v>2026-02-03T14:49:20.142Z</v>
       </c>
     </row>
     <row r="21">
@@ -1005,10 +1005,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H21" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I21" t="str">
-        <v>2026-02-03T14:07:13.664Z</v>
+        <v>2026-02-03T14:49:20.145Z</v>
       </c>
     </row>
     <row r="22">
@@ -1034,10 +1034,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H22" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I22" t="str">
-        <v>2026-02-03T14:07:13.666Z</v>
+        <v>2026-02-03T14:49:20.147Z</v>
       </c>
     </row>
     <row r="23">
@@ -1063,10 +1063,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H23" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I23" t="str">
-        <v>2026-02-03T14:07:13.671Z</v>
+        <v>2026-02-03T14:49:20.151Z</v>
       </c>
     </row>
     <row r="24">
@@ -1092,10 +1092,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H24" t="str">
-        <v>2026-02-03T14:07:13.576Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I24" t="str">
-        <v>2026-02-03T14:07:13.679Z</v>
+        <v>2026-02-03T14:49:20.158Z</v>
       </c>
     </row>
     <row r="25">
@@ -1121,10 +1121,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H25" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I25" t="str">
-        <v>2026-02-03T14:07:13.681Z</v>
+        <v>2026-02-03T14:49:20.160Z</v>
       </c>
     </row>
     <row r="26">
@@ -1150,10 +1150,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H26" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I26" t="str">
-        <v>2026-02-03T14:07:13.684Z</v>
+        <v>2026-02-03T14:49:20.162Z</v>
       </c>
     </row>
     <row r="27">
@@ -1179,10 +1179,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H27" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.050Z</v>
       </c>
       <c r="I27" t="str">
-        <v>2026-02-03T14:07:13.686Z</v>
+        <v>2026-02-03T14:49:20.165Z</v>
       </c>
     </row>
     <row r="28">
@@ -1208,10 +1208,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H28" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.051Z</v>
       </c>
       <c r="I28" t="str">
-        <v>2026-02-03T14:07:13.688Z</v>
+        <v>2026-02-03T14:49:20.167Z</v>
       </c>
     </row>
     <row r="29">
@@ -1237,10 +1237,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H29" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.051Z</v>
       </c>
       <c r="I29" t="str">
-        <v>2026-02-03T14:07:13.691Z</v>
+        <v>2026-02-03T14:49:20.170Z</v>
       </c>
     </row>
     <row r="30">
@@ -1266,10 +1266,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H30" t="str">
-        <v>2026-02-03T14:07:13.577Z</v>
+        <v>2026-02-03T14:49:20.051Z</v>
       </c>
       <c r="I30" t="str">
-        <v>2026-02-03T14:07:13.693Z</v>
+        <v>2026-02-03T14:49:20.173Z</v>
       </c>
     </row>
     <row r="31">
@@ -1295,10 +1295,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H31" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.051Z</v>
       </c>
       <c r="I31" t="str">
-        <v>2026-02-03T14:07:13.695Z</v>
+        <v>2026-02-03T14:49:20.175Z</v>
       </c>
     </row>
     <row r="32">
@@ -1324,10 +1324,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H32" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.051Z</v>
       </c>
       <c r="I32" t="str">
-        <v>2026-02-03T14:07:13.698Z</v>
+        <v>2026-02-03T14:49:20.178Z</v>
       </c>
     </row>
     <row r="33">
@@ -1353,10 +1353,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H33" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I33" t="str">
-        <v>2026-02-03T14:07:13.701Z</v>
+        <v>2026-02-03T14:49:20.180Z</v>
       </c>
     </row>
     <row r="34">
@@ -1382,10 +1382,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H34" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I34" t="str">
-        <v>2026-02-03T14:07:13.705Z</v>
+        <v>2026-02-03T14:49:20.182Z</v>
       </c>
     </row>
     <row r="35">
@@ -1411,10 +1411,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H35" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I35" t="str">
-        <v>2026-02-03T14:07:13.708Z</v>
+        <v>2026-02-03T14:49:20.185Z</v>
       </c>
     </row>
     <row r="36">
@@ -1440,10 +1440,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H36" t="str">
-        <v>2026-02-03T14:07:13.578Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I36" t="str">
-        <v>2026-02-03T14:07:13.710Z</v>
+        <v>2026-02-03T14:49:20.187Z</v>
       </c>
     </row>
     <row r="37">
@@ -1469,10 +1469,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H37" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I37" t="str">
-        <v>2026-02-03T14:07:13.713Z</v>
+        <v>2026-02-03T14:49:20.190Z</v>
       </c>
     </row>
     <row r="38">
@@ -1498,10 +1498,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H38" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I38" t="str">
-        <v>2026-02-03T14:07:13.720Z</v>
+        <v>2026-02-03T14:49:20.191Z</v>
       </c>
     </row>
     <row r="39">
@@ -1527,10 +1527,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H39" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.052Z</v>
       </c>
       <c r="I39" t="str">
-        <v>2026-02-03T14:07:13.722Z</v>
+        <v>2026-02-03T14:49:20.194Z</v>
       </c>
     </row>
     <row r="40">
@@ -1556,10 +1556,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H40" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I40" t="str">
-        <v>2026-02-03T14:07:13.724Z</v>
+        <v>2026-02-03T14:49:20.196Z</v>
       </c>
     </row>
     <row r="41">
@@ -1585,10 +1585,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H41" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I41" t="str">
-        <v>2026-02-03T14:07:13.726Z</v>
+        <v>2026-02-03T14:49:20.199Z</v>
       </c>
     </row>
     <row r="42">
@@ -1614,10 +1614,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H42" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I42" t="str">
-        <v>2026-02-03T14:07:13.728Z</v>
+        <v>2026-02-03T14:49:20.201Z</v>
       </c>
     </row>
     <row r="43">
@@ -1643,10 +1643,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H43" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I43" t="str">
-        <v>2026-02-03T14:07:13.730Z</v>
+        <v>2026-02-03T14:49:20.203Z</v>
       </c>
     </row>
     <row r="44">
@@ -1672,10 +1672,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H44" t="str">
-        <v>2026-02-03T14:07:13.579Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I44" t="str">
-        <v>2026-02-03T14:07:13.733Z</v>
+        <v>2026-02-03T14:49:20.205Z</v>
       </c>
     </row>
     <row r="45">
@@ -1701,10 +1701,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H45" t="str">
-        <v>2026-02-03T14:07:13.580Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I45" t="str">
-        <v>2026-02-03T14:07:13.736Z</v>
+        <v>2026-02-03T14:49:20.207Z</v>
       </c>
     </row>
     <row r="46">
@@ -1730,10 +1730,10 @@
         <v>Upcoming</v>
       </c>
       <c r="H46" t="str">
-        <v>2026-02-03T14:07:13.580Z</v>
+        <v>2026-02-03T14:49:20.053Z</v>
       </c>
       <c r="I46" t="str">
-        <v>2026-02-03T14:07:13.740Z</v>
+        <v>2026-02-03T14:49:20.215Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>